<commit_message>
Ajout d'un model pour le detail commande, resolution bug modif info perso utilisateurs, ajout d un fichier pour les taches restantes, ajout d un fichier excel pour le infos utilisateurs
</commit_message>
<xml_diff>
--- a/InfosUtilisateursSite.xlsx
+++ b/InfosUtilisateursSite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lemai\Documents\13_ProjetsPro\1_FormationDevWeb_2022_2023\Site_E-Commerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D7E182-A7EF-460C-8D1C-68F4E36DCA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A375F4-9DCE-401C-8720-8167A1F512CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -563,7 +563,7 @@
   <dimension ref="D2:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>